<commit_message>
basic game completed. needs work on exception handling
</commit_message>
<xml_diff>
--- a/src/main/resources/评分标准.xlsx
+++ b/src/main/resources/评分标准.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>要求</t>
   </si>
@@ -1473,8 +1473,8 @@
   <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1520,13 +1520,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="10">
         <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1636,13 +1639,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="28.8" spans="1:3">
+    <row r="14" ht="28.8" spans="1:4">
       <c r="A14" s="8"/>
       <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="10">
         <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">

</xml_diff>

<commit_message>
handle excpetion when server shuts down
</commit_message>
<xml_diff>
--- a/src/main/resources/评分标准.xlsx
+++ b/src/main/resources/评分标准.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>要求</t>
   </si>
@@ -1474,7 +1474,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1651,7 +1651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="13" t="s">
         <v>19</v>
       </c>
@@ -1660,6 +1660,9 @@
       </c>
       <c r="C15" s="10">
         <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">

</xml_diff>

<commit_message>
reslove the case that one player loses connection during game
</commit_message>
<xml_diff>
--- a/src/main/resources/评分标准.xlsx
+++ b/src/main/resources/评分标准.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>要求</t>
   </si>
@@ -1473,8 +1473,8 @@
   <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1665,12 +1665,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="10">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1725,13 +1728,16 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" ht="15.15" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="16">
         <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to resolve the matching time exception. not yet completed
</commit_message>
<xml_diff>
--- a/src/main/resources/评分标准.xlsx
+++ b/src/main/resources/评分标准.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>要求</t>
   </si>
@@ -117,6 +117,9 @@
     <t>客户端在等待匹配的过程中异常关闭，服务器能以合理的方式处理。</t>
   </si>
   <si>
+    <t>TODO</t>
+  </si>
+  <si>
     <t>当2个客户端都异常关闭，服务器应该解除该会话并记录log信息。</t>
   </si>
   <si>
@@ -127,9 +130,6 @@
   </si>
   <si>
     <t>账号管理系统，要求用户可以注册和登录账号，并查看自己和他人的游戏历史、是否在线等信息。</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>连接服务器后，玩家可以看到当前等待匹配的玩家列表。玩家可以从玩家列表中选择对手开始新游戏。</t>
@@ -1473,8 +1473,8 @@
   <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1677,7 +1677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="13"/>
       <c r="B17" s="11" t="s">
         <v>22</v>
@@ -1685,11 +1685,14 @@
       <c r="C17" s="10">
         <v>4</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="13"/>
       <c r="B18" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="10">
         <v>2</v>
@@ -1698,22 +1701,22 @@
     <row r="19" spans="1:3">
       <c r="A19" s="13"/>
       <c r="B19" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="10">
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1725,10 +1728,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" ht="15.15" spans="1:4">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
         <v>29</v>
@@ -1737,7 +1740,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
players can now view their game records
</commit_message>
<xml_diff>
--- a/src/main/resources/评分标准.xlsx
+++ b/src/main/resources/评分标准.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>要求</t>
   </si>
@@ -117,22 +117,22 @@
     <t>客户端在等待匹配的过程中异常关闭，服务器能以合理的方式处理。</t>
   </si>
   <si>
+    <t>当2个客户端都异常关闭，服务器应该解除该会话并记录log信息。</t>
+  </si>
+  <si>
+    <t>注：合理的方式可以是界面弹出错误提示信息或其他明显的提示方式。在console抛异常不计分。</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>账号管理系统，要求用户可以注册和登录账号，并查看自己和他人的游戏历史、是否在线等信息。</t>
+  </si>
+  <si>
+    <t>连接服务器后，玩家可以看到当前等待匹配的玩家列表。玩家可以从玩家列表中选择对手开始新游戏。</t>
+  </si>
+  <si>
     <t>TODO</t>
-  </si>
-  <si>
-    <t>当2个客户端都异常关闭，服务器应该解除该会话并记录log信息。</t>
-  </si>
-  <si>
-    <t>注：合理的方式可以是界面弹出错误提示信息或其他明显的提示方式。在console抛异常不计分。</t>
-  </si>
-  <si>
-    <t>Bonus</t>
-  </si>
-  <si>
-    <t>账号管理系统，要求用户可以注册和登录账号，并查看自己和他人的游戏历史、是否在线等信息。</t>
-  </si>
-  <si>
-    <t>连接服务器后，玩家可以看到当前等待匹配的玩家列表。玩家可以从玩家列表中选择对手开始新游戏。</t>
   </si>
   <si>
     <t>玩家在游戏中断后，可以重新连接到服务器并从之前的游戏状态和之前的对手继续游戏。</t>
@@ -1474,7 +1474,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1686,49 +1686,52 @@
         <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="13"/>
       <c r="B18" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="10">
         <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="13"/>
       <c r="B19" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="C20" s="10">
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="13"/>
       <c r="B21" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="10">
         <v>5</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" ht="15.15" spans="1:4">
@@ -1740,7 +1743,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>